<commit_message>
SentBy Changes in SMS, WhatsApp, Email
</commit_message>
<xml_diff>
--- a/Communication_API/EmailReport.xlsx
+++ b/Communication_API/EmailReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Admission Number</t>
   </si>
@@ -35,6 +35,9 @@
     <t>Status</t>
   </si>
   <si>
+    <t>Sent By</t>
+  </si>
+  <si>
     <t>ADM001</t>
   </si>
   <si>
@@ -44,13 +47,16 @@
     <t>Grade 1-Section A</t>
   </si>
   <si>
-    <t>19 January 2025, 12:00 AM</t>
+    <t>15 February 2025, 12:00 AM</t>
   </si>
   <si>
-    <t>Reminder: Upcoming Exams</t>
+    <t>Welcome to Our Institute</t>
   </si>
   <si>
-    <t>Delivered</t>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>John Smith</t>
   </si>
   <si>
     <t>ADM002</t>
@@ -59,7 +65,7 @@
     <t>Vivaan Raj Gupta</t>
   </si>
   <si>
-    <t>Pending</t>
+    <t>Exam Schedule Announcement</t>
   </si>
 </sst>
 </file>
@@ -106,7 +112,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -134,47 +140,56 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2"/>
       <c r="G2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F3"/>
       <c r="G3" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>